<commit_message>
Updated Code for Final Submission
</commit_message>
<xml_diff>
--- a/gowalla-compiled.xlsx
+++ b/gowalla-compiled.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Eigenvector" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -317,10 +317,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1207,7 +1207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>

</xml_diff>